<commit_message>
Optimaliseren van code + bug fix
</commit_message>
<xml_diff>
--- a/Afwezigheden.xlsx
+++ b/Afwezigheden.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\Jaar 2\WPL3\PIBO Tongeren\Projecten\AfwezigheidsScherm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F5A3C9-F239-4492-AB2E-8A85AFD5388D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0782324B-BA0D-4582-8A06-93B4D22EDBCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
-  <si>
-    <t>Afwezig</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Koen Wauters</t>
   </si>
@@ -36,13 +33,16 @@
     <t>Jos De Vos</t>
   </si>
   <si>
-    <t>Jos Lemmens</t>
-  </si>
-  <si>
     <t>Kurt Vrancken</t>
   </si>
   <si>
-    <t>Iemand Iemandsen</t>
+    <t>Jeff Kippers</t>
+  </si>
+  <si>
+    <t>Goran Deckers</t>
+  </si>
+  <si>
+    <t>AFWEZIGHEDEN LEERKRACHTEN</t>
   </si>
 </sst>
 </file>
@@ -73,26 +73,32 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="16"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="16"/>
-      <color rgb="FFFF0000"/>
+      <sz val="30"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -122,17 +128,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,94 +422,131 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="E1:G13"/>
+  <dimension ref="D1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" customWidth="1"/>
+    <col min="4" max="4" width="29.77734375" customWidth="1"/>
     <col min="5" max="5" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.88671875" customWidth="1"/>
+    <col min="7" max="7" width="10.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="4:7" x14ac:dyDescent="0.3">
       <c r="F1" s="1"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="F2" s="2"/>
+    <row r="2" spans="4:7" ht="112.8" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="D2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="4:7" x14ac:dyDescent="0.3">
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="5:7" ht="21" x14ac:dyDescent="0.4">
+    <row r="4" spans="4:7" ht="21" x14ac:dyDescent="0.4">
       <c r="E4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="5:7" ht="21" x14ac:dyDescent="0.4">
+    <row r="5" spans="4:7" ht="21" x14ac:dyDescent="0.4">
       <c r="E5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="4:7" ht="21" x14ac:dyDescent="0.4">
+      <c r="E6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>0</v>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="4:7" ht="21" x14ac:dyDescent="0.4">
+      <c r="E7" s="3" t="s">
+        <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="5:7" ht="21" x14ac:dyDescent="0.4">
-      <c r="E6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="5:7" ht="21" x14ac:dyDescent="0.4">
-      <c r="E7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="5:7" ht="21" x14ac:dyDescent="0.4">
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="4:7" ht="21" x14ac:dyDescent="0.4">
       <c r="E8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="5:7" ht="21" x14ac:dyDescent="0.4">
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="4:7" ht="21" x14ac:dyDescent="0.4">
       <c r="E9" s="3"/>
-      <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="5:7" ht="21" x14ac:dyDescent="0.4">
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="4:7" ht="21" x14ac:dyDescent="0.4">
       <c r="E10" s="3"/>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="5:7" ht="21" x14ac:dyDescent="0.4">
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="4:7" ht="21" x14ac:dyDescent="0.4">
       <c r="E11" s="3"/>
-      <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="5:7" ht="21" x14ac:dyDescent="0.4">
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="4:7" ht="21" x14ac:dyDescent="0.4">
       <c r="E12" s="3"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
+    <row r="13" spans="4:7" ht="21" x14ac:dyDescent="0.4">
+      <c r="E13" s="3"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="4:7" ht="21" x14ac:dyDescent="0.4">
+      <c r="E14" s="3"/>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="4:7" ht="21" x14ac:dyDescent="0.4">
+      <c r="E15" s="3"/>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="4:7" ht="21" x14ac:dyDescent="0.4">
+      <c r="E16" s="3"/>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="5:6" ht="21" x14ac:dyDescent="0.4">
+      <c r="E17" s="3"/>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="5:6" ht="21" x14ac:dyDescent="0.4">
+      <c r="E18" s="3"/>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="5:6" ht="21" x14ac:dyDescent="0.4">
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="5:6" ht="21" x14ac:dyDescent="0.4">
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="5:6" ht="21" x14ac:dyDescent="0.4">
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="5:6" ht="21" x14ac:dyDescent="0.4">
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="5:6" ht="21" x14ac:dyDescent="0.4">
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="5:6" ht="21" x14ac:dyDescent="0.4">
+      <c r="E24" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D2:F2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>